<commit_message>
[DollHouse] Add rooster sound. It must be at most 44.1kHz.
</commit_message>
<xml_diff>
--- a/doll-house/doc/resistors.xlsx
+++ b/doll-house/doc/resistors.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
   <si>
     <t>R1</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>Wybieram</t>
+  </si>
+  <si>
+    <t>Dźwięk</t>
+  </si>
+  <si>
+    <t>door bell</t>
+  </si>
+  <si>
+    <t>owl</t>
+  </si>
+  <si>
+    <t>rooster</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1067,7 @@
   <dimension ref="A2:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,9 +1077,10 @@
     <col min="6" max="6" width="11.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
     <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1092,7 +1105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1103,7 +1116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1111,7 +1124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>3</v>
       </c>
@@ -1133,8 +1146,11 @@
       <c r="J8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>0</v>
       </c>
@@ -1166,8 +1182,11 @@
         <f>$H10 - $I9</f>
         <v>25.086532951289396</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1.8</v>
       </c>
@@ -1200,7 +1219,7 @@
         <v>25.039399675608035</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>3.9</v>
       </c>
@@ -1233,7 +1252,7 @@
         <v>30.115362245543054</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>6.8</v>
       </c>
@@ -1266,7 +1285,7 @@
         <v>26.97249417249418</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1298,8 +1317,11 @@
         <f t="shared" si="0"/>
         <v>37.96107506950878</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>15</v>
       </c>
@@ -1332,7 +1354,7 @@
         <v>43.482302543507387</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>22</v>
       </c>
@@ -1365,7 +1387,7 @@
         <v>55.018877887788676</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>33</v>
       </c>
@@ -1590,6 +1612,9 @@
       <c r="I22">
         <f t="shared" si="2"/>
         <v>977.4545454545455</v>
+      </c>
+      <c r="M22" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">

</xml_diff>